<commit_message>
Update Nucleus BOM with different fuse holders.
</commit_message>
<xml_diff>
--- a/Modules/Nucleus/Nucleus_BOM.xlsx
+++ b/Modules/Nucleus/Nucleus_BOM.xlsx
@@ -673,9 +673,6 @@
     <t>Fuse Holder</t>
   </si>
   <si>
-    <t>https://www.tme.eu/hr/en/details/10207101009/pcb-fuseholders/littelfuse/</t>
-  </si>
-  <si>
     <t>https://github.com/Thorinair/Avalon-Harmonics/blob/master/Modules/Nucleus/printable/Nucleus_Front.stl</t>
   </si>
   <si>
@@ -783,6 +780,9 @@
   </si>
   <si>
     <t>https://www.rhelectronics.store/high-voltage-geiger-probe-driver-power-supply-module-420v-550v-with-ttl-digitized-pulse-output</t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/Littelfuse/01240061H?qs=81r%252BiQLm7BSgqEC6g%252BUS9Q%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -1805,7 +1805,7 @@
   <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2006,7 +2006,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>41</v>
@@ -2015,7 +2015,7 @@
         <v>65</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2206,7 +2206,7 @@
         <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>50</v>
@@ -2215,7 +2215,7 @@
         <v>146</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -2229,10 +2229,10 @@
         <v>48</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>88</v>
@@ -2547,13 +2547,13 @@
         <v>153</v>
       </c>
       <c r="C41" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E41" t="s">
         <v>154</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>155</v>
+        <v>178</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -2579,7 +2579,7 @@
         <v>3</v>
       </c>
       <c r="B44" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C44" t="s">
         <v>112</v>
@@ -2588,7 +2588,7 @@
         <v>145</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -2613,16 +2613,16 @@
         <v>1</v>
       </c>
       <c r="B46" t="s">
+        <v>169</v>
+      </c>
+      <c r="C46" t="s">
         <v>170</v>
-      </c>
-      <c r="C46" t="s">
-        <v>171</v>
       </c>
       <c r="E46" t="s">
         <v>110</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -2636,7 +2636,7 @@
         <v>142</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -2650,7 +2650,7 @@
         <v>141</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -2660,17 +2660,17 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B53" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B54" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B55" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -2686,7 +2686,7 @@
         <v>127</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -2697,7 +2697,7 @@
         <v>128</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2708,7 +2708,7 @@
         <v>129</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -2719,15 +2719,15 @@
         <v>140</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add SBM-20 as valid tube to BOM.
</commit_message>
<xml_diff>
--- a/Modules/Nucleus/Nucleus_BOM.xlsx
+++ b/Modules/Nucleus/Nucleus_BOM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="181">
   <si>
     <t>Qty</t>
   </si>
@@ -601,9 +601,6 @@
     <t>High Voltage Power Supply Module for 400V 500V Geiger Tube</t>
   </si>
   <si>
-    <t>STS-5 Geiger Muller Counter Tube</t>
-  </si>
-  <si>
     <t>https://www.tme.eu/hr/en/details/nsr-03/pin-headers/ninigi/</t>
   </si>
   <si>
@@ -783,6 +780,15 @@
   </si>
   <si>
     <t>https://hr.mouser.com/ProductDetail/Littelfuse/01240061H?qs=81r%252BiQLm7BSgqEC6g%252BUS9Q%3D%3D</t>
+  </si>
+  <si>
+    <t>Geiger Muller Counter Tube (SBM-20 or STS-5)</t>
+  </si>
+  <si>
+    <t>https://soviet-tubes.com/product/sbm20-sbm-20-geiger-muller-counter-is-designed-to-detect-hard-beta-and-gamma-radiation-in-radio-engineering-devices/</t>
+  </si>
+  <si>
+    <t>https://www.ebay.co.uk/itm/222197033139</t>
   </si>
 </sst>
 </file>
@@ -1802,10 +1808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U57" sqref="U57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1835,7 +1841,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2006,7 +2012,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>41</v>
@@ -2015,7 +2021,7 @@
         <v>65</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2206,16 +2212,16 @@
         <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>50</v>
       </c>
       <c r="E20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -2229,10 +2235,10 @@
         <v>48</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>88</v>
@@ -2312,7 +2318,7 @@
         <v>25</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2417,7 +2423,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>4</v>
       </c>
@@ -2434,7 +2440,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>4</v>
       </c>
@@ -2451,7 +2457,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>4</v>
       </c>
@@ -2468,27 +2474,27 @@
         <v>125</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F36" s="7"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C37" t="s">
         <v>149</v>
       </c>
-      <c r="C37" t="s">
-        <v>150</v>
-      </c>
       <c r="E37" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1</v>
       </c>
@@ -2496,16 +2502,16 @@
         <v>95</v>
       </c>
       <c r="C38" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E38" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1</v>
       </c>
@@ -2513,85 +2519,85 @@
         <v>96</v>
       </c>
       <c r="C39" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E39" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>5</v>
       </c>
       <c r="B40" t="s">
+        <v>136</v>
+      </c>
+      <c r="C40" t="s">
+        <v>134</v>
+      </c>
+      <c r="E40" t="s">
         <v>137</v>
       </c>
-      <c r="C40" t="s">
-        <v>135</v>
-      </c>
-      <c r="E40" t="s">
-        <v>138</v>
-      </c>
       <c r="F40" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2</v>
       </c>
       <c r="B41" t="s">
+        <v>152</v>
+      </c>
+      <c r="C41" t="s">
+        <v>172</v>
+      </c>
+      <c r="E41" t="s">
         <v>153</v>
       </c>
-      <c r="C41" t="s">
-        <v>173</v>
-      </c>
-      <c r="E41" t="s">
-        <v>154</v>
-      </c>
       <c r="F41" s="7" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B42" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C42" t="s">
+        <v>142</v>
+      </c>
+      <c r="E42" t="s">
         <v>143</v>
       </c>
-      <c r="E42" t="s">
-        <v>144</v>
-      </c>
       <c r="F42" s="7"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F43" s="7"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>3</v>
       </c>
       <c r="B44" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C44" t="s">
         <v>112</v>
       </c>
       <c r="E44" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1</v>
       </c>
@@ -2608,24 +2614,24 @@
         <v>114</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1</v>
       </c>
       <c r="B46" t="s">
+        <v>168</v>
+      </c>
+      <c r="C46" t="s">
         <v>169</v>
-      </c>
-      <c r="C46" t="s">
-        <v>170</v>
       </c>
       <c r="E46" t="s">
         <v>110</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1</v>
       </c>
@@ -2633,52 +2639,58 @@
         <v>130</v>
       </c>
       <c r="E48" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+      <c r="K48" s="7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1</v>
       </c>
       <c r="B49" t="s">
-        <v>131</v>
+        <v>178</v>
       </c>
       <c r="E49" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+      <c r="K49" s="7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B53" s="9" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B54" s="9" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B55" s="9" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>1</v>
       </c>
@@ -2686,10 +2698,10 @@
         <v>127</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>1</v>
       </c>
@@ -2697,10 +2709,10 @@
         <v>128</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>1</v>
       </c>
@@ -2708,26 +2720,26 @@
         <v>129</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>1</v>
       </c>
       <c r="B61" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B63" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -2769,10 +2781,12 @@
     <hyperlink ref="F46" r:id="rId35"/>
     <hyperlink ref="F49" r:id="rId36"/>
     <hyperlink ref="F20" r:id="rId37"/>
-    <hyperlink ref="F48" r:id="rId38"/>
+    <hyperlink ref="K49" r:id="rId38"/>
+    <hyperlink ref="F48" r:id="rId39"/>
+    <hyperlink ref="K48" r:id="rId40"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId39"/>
-  <drawing r:id="rId40"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId41"/>
+  <drawing r:id="rId42"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add buy link for SubMini switch washers.
</commit_message>
<xml_diff>
--- a/Modules/Nucleus/Nucleus_BOM.xlsx
+++ b/Modules/Nucleus/Nucleus_BOM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="184">
   <si>
     <t>Qty</t>
   </si>
@@ -795,6 +795,9 @@
   </si>
   <si>
     <t>https://avalonharmonics.etsy.com/listing/1627685702/printed-parts-avalon-harmonics-nucleus</t>
+  </si>
+  <si>
+    <t>https://avalonharmonics.etsy.com/uk/listing/1640523986/printed-parts-20x-submini-switch-washers</t>
   </si>
 </sst>
 </file>
@@ -1817,7 +1820,7 @@
   <dimension ref="A1:O63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L61" sqref="L61"/>
+      <selection activeCell="N53" sqref="N53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2756,6 +2759,12 @@
       </c>
       <c r="C61" s="7" t="s">
         <v>157</v>
+      </c>
+      <c r="L61" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="O61" s="7" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
@@ -2808,9 +2817,13 @@
     <hyperlink ref="K49" r:id="rId38"/>
     <hyperlink ref="F48" r:id="rId39"/>
     <hyperlink ref="K48" r:id="rId40"/>
+    <hyperlink ref="O61" r:id="rId41"/>
+    <hyperlink ref="O58" r:id="rId42"/>
+    <hyperlink ref="O59" r:id="rId43"/>
+    <hyperlink ref="O60" r:id="rId44"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId41"/>
-  <drawing r:id="rId42"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId45"/>
+  <drawing r:id="rId46"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Upgrade Nucleus to 1.2, fix triggers not working.
</commit_message>
<xml_diff>
--- a/Modules/Nucleus/Nucleus_BOM.xlsx
+++ b/Modules/Nucleus/Nucleus_BOM.xlsx
@@ -1,20 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My-Dev\Modular Synth\Avalon Harmonics\Nucleus\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB01C3C-9FFF-49BC-96A1-DA2B6DF5FB5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="690" windowWidth="36915" windowHeight="17385"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nucleus" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="185">
   <si>
     <t>Qty</t>
   </si>
@@ -234,23 +253,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>R6</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>R1,</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> R5</t>
     </r>
   </si>
   <si>
@@ -799,11 +801,17 @@
   <si>
     <t>https://avalonharmonics.etsy.com/uk/listing/1640523986/printed-parts-20x-submini-switch-washers</t>
   </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1433,6 +1441,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1443,18 +1454,24 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>819150</xdr:colOff>
-      <xdr:row>89</xdr:row>
+      <xdr:row>90</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1487,18 +1504,24 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>91</xdr:row>
+      <xdr:row>92</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1531,9 +1554,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1571,7 +1594,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1643,7 +1666,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1816,11 +1839,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O63"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N53" sqref="N53"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1850,107 +1873,107 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>220</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
         <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>183</v>
       </c>
       <c r="E2" t="s">
         <v>32</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>220</v>
       </c>
       <c r="C3" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>71</v>
+      <c r="D3" s="5" t="s">
+        <v>184</v>
       </c>
       <c r="E3" t="s">
         <v>32</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
         <v>30</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="6" t="s">
         <v>70</v>
       </c>
       <c r="E4" t="s">
         <v>32</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
         <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E5" t="s">
         <v>32</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>31</v>
+      <c r="D6" t="s">
+        <v>68</v>
       </c>
       <c r="E6" t="s">
         <v>32</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1958,19 +1981,19 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" t="s">
-        <v>35</v>
+        <v>30</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1978,59 +2001,59 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>38</v>
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="E9" t="s">
         <v>64</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>41</v>
+        <v>6</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>71</v>
       </c>
       <c r="E10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>158</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2038,19 +2061,19 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" t="s">
-        <v>42</v>
+        <v>8</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="E11" t="s">
         <v>65</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>80</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2058,59 +2081,59 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E12" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D13" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="E13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="D14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E14" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2121,16 +2144,16 @@
         <v>61</v>
       </c>
       <c r="C15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>75</v>
+        <v>60</v>
+      </c>
+      <c r="D15" t="s">
+        <v>73</v>
       </c>
       <c r="E15" t="s">
         <v>61</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -2138,39 +2161,39 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>74</v>
       </c>
       <c r="E16" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>51</v>
+        <v>58</v>
+      </c>
+      <c r="D17" t="s">
+        <v>73</v>
       </c>
       <c r="E17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2178,19 +2201,19 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s">
         <v>57</v>
       </c>
-      <c r="D18" t="s">
-        <v>52</v>
+      <c r="D18" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="E18" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -2198,19 +2221,19 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E19" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -2218,96 +2241,99 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>170</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>50</v>
+        <v>62</v>
+      </c>
+      <c r="D20" t="s">
+        <v>53</v>
       </c>
       <c r="E20" t="s">
-        <v>145</v>
+        <v>56</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>171</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>48</v>
+        <v>169</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>163</v>
+        <v>50</v>
       </c>
       <c r="E21" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>88</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="C22" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>34</v>
+        <v>162</v>
       </c>
       <c r="E22" t="s">
-        <v>63</v>
+        <v>160</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="C23" t="s">
-        <v>90</v>
+        <v>33</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="E23" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="C24" t="s">
-        <v>93</v>
-      </c>
-      <c r="D24" t="s">
-        <v>26</v>
+        <v>89</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="E24" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2315,36 +2341,36 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C25" t="s">
         <v>92</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>29</v>
+      <c r="D25" t="s">
+        <v>26</v>
       </c>
       <c r="E25" t="s">
         <v>25</v>
       </c>
-      <c r="F25" s="7" t="s">
-        <v>150</v>
-      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C26" t="s">
-        <v>93</v>
-      </c>
-      <c r="D26" t="s">
-        <v>27</v>
+        <v>91</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="E26" t="s">
         <v>25</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2352,13 +2378,13 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E27" t="s">
         <v>25</v>
@@ -2369,33 +2395,33 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D28" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E28" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>2</v>
-      </c>
-      <c r="B30" t="s">
-        <v>98</v>
-      </c>
-      <c r="C30" t="s">
-        <v>99</v>
-      </c>
-      <c r="E30" t="s">
-        <v>100</v>
-      </c>
-      <c r="F30" s="7" t="s">
-        <v>101</v>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -2403,16 +2429,16 @@
         <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C31" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E31" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -2420,241 +2446,241 @@
         <v>2</v>
       </c>
       <c r="B32" t="s">
+        <v>101</v>
+      </c>
+      <c r="C32" t="s">
+        <v>102</v>
+      </c>
+      <c r="E32" t="s">
+        <v>103</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>2</v>
+      </c>
+      <c r="B33" t="s">
+        <v>105</v>
+      </c>
+      <c r="C33" t="s">
         <v>106</v>
       </c>
-      <c r="C32" t="s">
+      <c r="E33" t="s">
         <v>107</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F33" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="F32" s="7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>4</v>
-      </c>
-      <c r="B33" t="s">
-        <v>116</v>
-      </c>
-      <c r="C33" t="s">
-        <v>117</v>
-      </c>
-      <c r="E33" t="s">
-        <v>120</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>4</v>
       </c>
       <c r="B34" t="s">
+        <v>115</v>
+      </c>
+      <c r="C34" t="s">
+        <v>116</v>
+      </c>
+      <c r="E34" t="s">
         <v>119</v>
       </c>
-      <c r="C34" t="s">
+      <c r="F34" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="E34" t="s">
-        <v>121</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>4</v>
       </c>
       <c r="B35" t="s">
+        <v>118</v>
+      </c>
+      <c r="C35" t="s">
+        <v>116</v>
+      </c>
+      <c r="E35" t="s">
+        <v>120</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>4</v>
+      </c>
+      <c r="B36" t="s">
+        <v>122</v>
+      </c>
+      <c r="C36" t="s">
+        <v>116</v>
+      </c>
+      <c r="E36" t="s">
         <v>123</v>
       </c>
-      <c r="C35" t="s">
-        <v>117</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="F36" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="F35" s="7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F36" s="7"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>1</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C37" t="s">
-        <v>149</v>
-      </c>
-      <c r="E37" t="s">
-        <v>147</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1</v>
       </c>
-      <c r="B38" t="s">
-        <v>95</v>
+      <c r="B38" s="1" t="s">
+        <v>147</v>
       </c>
       <c r="C38" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="E38" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C39" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E39" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
       <c r="C40" t="s">
         <v>134</v>
       </c>
       <c r="E40" t="s">
+        <v>136</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>5</v>
+      </c>
+      <c r="B41" t="s">
+        <v>135</v>
+      </c>
+      <c r="C41" t="s">
+        <v>133</v>
+      </c>
+      <c r="E41" t="s">
+        <v>136</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="B42" t="s">
+        <v>151</v>
+      </c>
+      <c r="C42" t="s">
+        <v>171</v>
+      </c>
+      <c r="E42" t="s">
+        <v>152</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="F40" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>2</v>
-      </c>
-      <c r="B41" t="s">
-        <v>152</v>
-      </c>
-      <c r="C41" t="s">
-        <v>172</v>
-      </c>
-      <c r="E41" t="s">
-        <v>153</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="B42" t="s">
-        <v>136</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="B43" t="s">
+        <v>135</v>
+      </c>
+      <c r="C43" t="s">
+        <v>141</v>
+      </c>
+      <c r="E43" t="s">
         <v>142</v>
       </c>
-      <c r="E42" t="s">
+      <c r="F43" s="7"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F44" s="7"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>3</v>
+      </c>
+      <c r="B45" t="s">
+        <v>163</v>
+      </c>
+      <c r="C45" t="s">
+        <v>111</v>
+      </c>
+      <c r="E45" t="s">
         <v>143</v>
       </c>
-      <c r="F42" s="7"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F43" s="7"/>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>3</v>
-      </c>
-      <c r="B44" t="s">
+      <c r="F45" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="C44" t="s">
-        <v>112</v>
-      </c>
-      <c r="E44" t="s">
-        <v>144</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>1</v>
-      </c>
-      <c r="B45" t="s">
-        <v>111</v>
-      </c>
-      <c r="C45" t="s">
-        <v>115</v>
-      </c>
-      <c r="E45" t="s">
-        <v>113</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1</v>
       </c>
       <c r="B46" t="s">
+        <v>110</v>
+      </c>
+      <c r="C46" t="s">
+        <v>114</v>
+      </c>
+      <c r="E46" t="s">
+        <v>112</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47" t="s">
+        <v>167</v>
+      </c>
+      <c r="C47" t="s">
         <v>168</v>
       </c>
-      <c r="C46" t="s">
-        <v>169</v>
-      </c>
-      <c r="E46" t="s">
-        <v>110</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>1</v>
-      </c>
-      <c r="B48" t="s">
-        <v>130</v>
-      </c>
-      <c r="E48" t="s">
-        <v>141</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="K48" s="7" t="s">
-        <v>176</v>
+      <c r="E47" t="s">
+        <v>109</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
@@ -2662,26 +2688,38 @@
         <v>1</v>
       </c>
       <c r="B49" t="s">
-        <v>178</v>
+        <v>129</v>
       </c>
       <c r="E49" t="s">
         <v>140</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>167</v>
+        <v>179</v>
       </c>
       <c r="K49" s="7" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B51" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="B50" t="s">
+        <v>177</v>
+      </c>
+      <c r="E50" t="s">
+        <v>139</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="K50" s="7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B52" s="5" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B53" s="9" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
@@ -2691,29 +2729,17 @@
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B55" s="9" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
-        <v>126</v>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B56" s="9" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>1</v>
-      </c>
-      <c r="B58" t="s">
-        <v>127</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="L58" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="O58" s="7" t="s">
-        <v>182</v>
+      <c r="A58" s="4" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
@@ -2721,16 +2747,16 @@
         <v>1</v>
       </c>
       <c r="B59" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="L59" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="O59" s="7" t="s">
         <v>181</v>
-      </c>
-      <c r="O59" s="7" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
@@ -2738,16 +2764,16 @@
         <v>1</v>
       </c>
       <c r="B60" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="L60" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="O60" s="7" t="s">
         <v>181</v>
-      </c>
-      <c r="O60" s="7" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
@@ -2755,75 +2781,93 @@
         <v>1</v>
       </c>
       <c r="B61" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L61" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="O61" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="O61" s="7" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B63" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="E63" s="4" t="s">
-        <v>173</v>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="B62" t="s">
+        <v>138</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="L62" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="O62" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B64" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2:F6" r:id="rId1" display="https://www.aliexpress.com/item/1005002670881002.html"/>
-    <hyperlink ref="F7" r:id="rId2"/>
-    <hyperlink ref="F8" r:id="rId3"/>
-    <hyperlink ref="F9" r:id="rId4"/>
-    <hyperlink ref="F11" r:id="rId5"/>
-    <hyperlink ref="F12" r:id="rId6"/>
-    <hyperlink ref="F13" r:id="rId7"/>
-    <hyperlink ref="F14" r:id="rId8"/>
-    <hyperlink ref="F15" r:id="rId9"/>
-    <hyperlink ref="F16" r:id="rId10"/>
-    <hyperlink ref="F17" r:id="rId11"/>
-    <hyperlink ref="F18" r:id="rId12"/>
-    <hyperlink ref="F19" r:id="rId13"/>
-    <hyperlink ref="F21" r:id="rId14"/>
-    <hyperlink ref="F22" r:id="rId15"/>
-    <hyperlink ref="F23" r:id="rId16"/>
-    <hyperlink ref="F30" r:id="rId17"/>
-    <hyperlink ref="F31" r:id="rId18"/>
-    <hyperlink ref="F32" r:id="rId19"/>
-    <hyperlink ref="F33" r:id="rId20"/>
-    <hyperlink ref="F34" r:id="rId21"/>
-    <hyperlink ref="F35" r:id="rId22"/>
-    <hyperlink ref="C58" r:id="rId23"/>
-    <hyperlink ref="C59" r:id="rId24"/>
-    <hyperlink ref="C60" r:id="rId25"/>
-    <hyperlink ref="F38" r:id="rId26"/>
-    <hyperlink ref="F39" r:id="rId27"/>
-    <hyperlink ref="F40" r:id="rId28"/>
-    <hyperlink ref="C61" r:id="rId29"/>
-    <hyperlink ref="F37" r:id="rId30"/>
-    <hyperlink ref="F25" r:id="rId31"/>
-    <hyperlink ref="F45" r:id="rId32"/>
-    <hyperlink ref="F41" r:id="rId33"/>
-    <hyperlink ref="F44" r:id="rId34"/>
-    <hyperlink ref="F46" r:id="rId35"/>
-    <hyperlink ref="F49" r:id="rId36"/>
-    <hyperlink ref="F20" r:id="rId37"/>
-    <hyperlink ref="K49" r:id="rId38"/>
-    <hyperlink ref="F48" r:id="rId39"/>
-    <hyperlink ref="K48" r:id="rId40"/>
-    <hyperlink ref="O61" r:id="rId41"/>
-    <hyperlink ref="O58" r:id="rId42"/>
-    <hyperlink ref="O59" r:id="rId43"/>
-    <hyperlink ref="O60" r:id="rId44"/>
+    <hyperlink ref="F3:F7" r:id="rId1" display="https://www.aliexpress.com/item/1005002670881002.html" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F8" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F9" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F10" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F12" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F13" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F14" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="F15" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F16" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="F17" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="F18" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="F19" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="F20" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="F22" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="F23" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="F24" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="F31" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="F32" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="F33" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="F34" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="F35" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="F36" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="C59" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="C60" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="C61" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="F39" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="F40" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="F41" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="C62" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="F38" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="F26" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="F46" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="F42" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="F45" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="F47" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="F50" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="F21" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="K50" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="F49" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="K49" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="O62" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="O59" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="O60" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="O61" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="F2" r:id="rId45" xr:uid="{DD0C5450-CE7D-49B7-8A3D-BBCECC2ABEC5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId45"/>
-  <drawing r:id="rId46"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId46"/>
+  <drawing r:id="rId47"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Nucleus for fast op amps.
</commit_message>
<xml_diff>
--- a/Modules/Nucleus/Nucleus_BOM.xlsx
+++ b/Modules/Nucleus/Nucleus_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My-Dev\Modular Synth\Avalon Harmonics\Nucleus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB01C3C-9FFF-49BC-96A1-DA2B6DF5FB5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32603B76-ADD4-4C82-AAFA-A54F2A4F2B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="191">
   <si>
     <t>Qty</t>
   </si>
@@ -687,9 +687,6 @@
     <t>https://www.thonk.co.uk/shop/eurorack-diy-essentials/</t>
   </si>
   <si>
-    <t>** One LED is used for the printed case.</t>
-  </si>
-  <si>
     <t>* Needs to be a low profile capacitor, max height of 8mm.</t>
   </si>
   <si>
@@ -712,6 +709,69 @@
     </r>
   </si>
   <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>https://pushermanproductions.com/product/pushernuts-gold-smooth-edge-jack-nuts-pack-of-25/</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/32965476651.html</t>
+  </si>
+  <si>
+    <t>https://www.ebay.co.uk/itm/185419609093</t>
+  </si>
+  <si>
+    <t>Black 6.35mm-Round</t>
+  </si>
+  <si>
+    <t>Aliexpress Knob 15mm</t>
+  </si>
+  <si>
+    <t>Pot 9mm Alpha 6.35mm</t>
+  </si>
+  <si>
+    <t>https://www.thonk.co.uk/shop/alpha-9mm-pots/</t>
+  </si>
+  <si>
+    <t>Wiring Diagram</t>
+  </si>
+  <si>
+    <t>Remove these end stoppers and leg on fuse holders!</t>
+  </si>
+  <si>
+    <t>https://www.rhelectronics.store/high-voltage-geiger-probe-driver-power-supply-module-420v-550v-with-ttl-digitized-pulse-output</t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/Littelfuse/01240061H?qs=81r%252BiQLm7BSgqEC6g%252BUS9Q%3D%3D</t>
+  </si>
+  <si>
+    <t>Geiger Muller Counter Tube (SBM-20 or STS-5)</t>
+  </si>
+  <si>
+    <t>https://soviet-tubes.com/product/sbm20-sbm-20-geiger-muller-counter-is-designed-to-detect-hard-beta-and-gamma-radiation-in-radio-engineering-devices/</t>
+  </si>
+  <si>
+    <t>https://www.ebay.co.uk/itm/222197033139</t>
+  </si>
+  <si>
+    <t>Purchase in Etsy Store:</t>
+  </si>
+  <si>
+    <t>https://avalonharmonics.etsy.com/listing/1627685702/printed-parts-avalon-harmonics-nucleus</t>
+  </si>
+  <si>
+    <t>https://avalonharmonics.etsy.com/uk/listing/1640523986/printed-parts-20x-submini-switch-washers</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>LM358P</t>
+  </si>
+  <si>
     <r>
       <t>LD_CLICK, LD_GATE, LD_TRIG</t>
     </r>
@@ -725,32 +785,8 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>**</t>
+      <t>***</t>
     </r>
-  </si>
-  <si>
-    <t>Gold</t>
-  </si>
-  <si>
-    <t>https://pushermanproductions.com/product/pushernuts-gold-smooth-edge-jack-nuts-pack-of-25/</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/32965476651.html</t>
-  </si>
-  <si>
-    <t>https://www.ebay.co.uk/itm/185419609093</t>
-  </si>
-  <si>
-    <t>Black 6.35mm-Round</t>
-  </si>
-  <si>
-    <t>Aliexpress Knob 15mm</t>
-  </si>
-  <si>
-    <t>Pot 9mm Alpha 6.35mm</t>
-  </si>
-  <si>
-    <t>https://www.thonk.co.uk/shop/alpha-9mm-pots/</t>
   </si>
   <si>
     <r>
@@ -765,47 +801,41 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>***</t>
+      <t>****</t>
     </r>
   </si>
   <si>
-    <t>Wiring Diagram</t>
-  </si>
-  <si>
-    <t>*** The end stoppers on the fuse holders need to be cut off with flush cutters. This saves 1.4mm of vertical internal height, making the module easier to install. The leg on the side of the cut should be removed too. See photo below!</t>
-  </si>
-  <si>
-    <t>Remove these end stoppers and leg on fuse holders!</t>
-  </si>
-  <si>
-    <t>https://www.rhelectronics.store/high-voltage-geiger-probe-driver-power-supply-module-420v-550v-with-ttl-digitized-pulse-output</t>
-  </si>
-  <si>
-    <t>https://hr.mouser.com/ProductDetail/Littelfuse/01240061H?qs=81r%252BiQLm7BSgqEC6g%252BUS9Q%3D%3D</t>
-  </si>
-  <si>
-    <t>Geiger Muller Counter Tube (SBM-20 or STS-5)</t>
-  </si>
-  <si>
-    <t>https://soviet-tubes.com/product/sbm20-sbm-20-geiger-muller-counter-is-designed-to-detect-hard-beta-and-gamma-radiation-in-radio-engineering-devices/</t>
-  </si>
-  <si>
-    <t>https://www.ebay.co.uk/itm/222197033139</t>
-  </si>
-  <si>
-    <t>Purchase in Etsy Store:</t>
-  </si>
-  <si>
-    <t>https://avalonharmonics.etsy.com/listing/1627685702/printed-parts-avalon-harmonics-nucleus</t>
-  </si>
-  <si>
-    <t>https://avalonharmonics.etsy.com/uk/listing/1640523986/printed-parts-20x-submini-switch-washers</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>R5</t>
+    <t>**** The end stoppers on the fuse holders need to be cut off with flush cutters. This saves 1.4mm of vertical internal height, making the module easier to install. The leg on the side of the cut should be removed too. See photo below!</t>
+  </si>
+  <si>
+    <t>*** One LED is used for the printed case.</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/hr/en/details/lm358p/tht-operational-amplifiers/texas-instruments/</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <r>
+      <t>U1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>**</t>
+    </r>
+  </si>
+  <si>
+    <t>** Needs to be an LM358P with a very fast slew rate. 0.3V/us works best, otherwise performance of the module is highly unstable.</t>
+  </si>
+  <si>
+    <t>Dual Op Amp FAST</t>
   </si>
 </sst>
 </file>
@@ -1454,13 +1484,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>819150</xdr:colOff>
-      <xdr:row>90</xdr:row>
+      <xdr:row>92</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1504,13 +1534,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>92</xdr:row>
+      <xdr:row>94</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1840,10 +1870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O64"/>
+  <dimension ref="A1:O66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1887,7 +1917,7 @@
         <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E2" t="s">
         <v>32</v>
@@ -1907,7 +1937,7 @@
         <v>30</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E3" t="s">
         <v>32</v>
@@ -2064,7 +2094,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>41</v>
@@ -2178,22 +2208,22 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>181</v>
       </c>
       <c r="C17" t="s">
         <v>58</v>
       </c>
       <c r="D17" t="s">
-        <v>73</v>
+        <v>188</v>
       </c>
       <c r="E17" t="s">
-        <v>55</v>
+        <v>190</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>83</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2201,19 +2231,19 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>51</v>
+        <v>187</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -2221,19 +2251,19 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
         <v>57</v>
       </c>
-      <c r="D19" t="s">
-        <v>52</v>
+      <c r="D19" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="E19" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -2241,19 +2271,19 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E20" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -2261,96 +2291,99 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>169</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>50</v>
+        <v>62</v>
+      </c>
+      <c r="D21" t="s">
+        <v>53</v>
       </c>
       <c r="E21" t="s">
-        <v>144</v>
+        <v>56</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>170</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>167</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>162</v>
+        <v>50</v>
       </c>
       <c r="E22" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>87</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>34</v>
+        <v>182</v>
       </c>
       <c r="E23" t="s">
-        <v>63</v>
+        <v>159</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="C24" t="s">
-        <v>89</v>
+        <v>33</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="E24" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C25" t="s">
-        <v>92</v>
-      </c>
-      <c r="D25" t="s">
-        <v>26</v>
+        <v>89</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="E25" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2361,33 +2394,33 @@
         <v>93</v>
       </c>
       <c r="C26" t="s">
-        <v>91</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>29</v>
+        <v>92</v>
+      </c>
+      <c r="D26" t="s">
+        <v>26</v>
       </c>
       <c r="E26" t="s">
         <v>25</v>
       </c>
-      <c r="F26" s="7" t="s">
-        <v>149</v>
-      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C27" t="s">
-        <v>92</v>
-      </c>
-      <c r="D27" t="s">
-        <v>27</v>
+        <v>91</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="E27" t="s">
         <v>25</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -2395,13 +2428,13 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C28" t="s">
         <v>92</v>
       </c>
       <c r="D28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E28" t="s">
         <v>25</v>
@@ -2412,33 +2445,33 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C29" t="s">
         <v>92</v>
       </c>
       <c r="D29" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E29" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>2</v>
-      </c>
-      <c r="B31" t="s">
-        <v>97</v>
-      </c>
-      <c r="C31" t="s">
-        <v>98</v>
-      </c>
-      <c r="E31" t="s">
-        <v>99</v>
-      </c>
-      <c r="F31" s="7" t="s">
-        <v>100</v>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -2446,16 +2479,16 @@
         <v>2</v>
       </c>
       <c r="B32" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C32" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E32" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2463,33 +2496,33 @@
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C33" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E33" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="C34" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="E34" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -2497,16 +2530,16 @@
         <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C35" t="s">
         <v>116</v>
       </c>
       <c r="E35" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2514,53 +2547,53 @@
         <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C36" t="s">
         <v>116</v>
       </c>
       <c r="E36" t="s">
+        <v>120</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>4</v>
+      </c>
+      <c r="B37" t="s">
+        <v>122</v>
+      </c>
+      <c r="C37" t="s">
+        <v>116</v>
+      </c>
+      <c r="E37" t="s">
         <v>123</v>
       </c>
-      <c r="F36" s="7" t="s">
+      <c r="F37" s="7" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F37" s="7"/>
-    </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>1</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C38" t="s">
-        <v>148</v>
-      </c>
-      <c r="E38" t="s">
-        <v>146</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>145</v>
-      </c>
+      <c r="F38" s="7"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1</v>
       </c>
-      <c r="B39" t="s">
-        <v>94</v>
+      <c r="B39" s="1" t="s">
+        <v>147</v>
       </c>
       <c r="C39" t="s">
-        <v>134</v>
+        <v>148</v>
       </c>
       <c r="E39" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>130</v>
+        <v>145</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2568,7 +2601,7 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C40" t="s">
         <v>134</v>
@@ -2577,93 +2610,93 @@
         <v>136</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>135</v>
+        <v>95</v>
       </c>
       <c r="C41" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E41" t="s">
         <v>136</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
+        <v>5</v>
+      </c>
+      <c r="B42" t="s">
+        <v>135</v>
+      </c>
+      <c r="C42" t="s">
+        <v>133</v>
+      </c>
+      <c r="E42" t="s">
+        <v>136</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43">
         <v>2</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>151</v>
       </c>
-      <c r="C42" t="s">
-        <v>171</v>
-      </c>
-      <c r="E42" t="s">
+      <c r="C43" t="s">
+        <v>183</v>
+      </c>
+      <c r="E43" t="s">
         <v>152</v>
       </c>
-      <c r="F42" s="7" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
+      <c r="F43" s="7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>135</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>141</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E44" t="s">
         <v>142</v>
       </c>
-      <c r="F43" s="7"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F44" s="7"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>3</v>
-      </c>
-      <c r="B45" t="s">
-        <v>163</v>
-      </c>
-      <c r="C45" t="s">
-        <v>111</v>
-      </c>
-      <c r="E45" t="s">
-        <v>143</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>164</v>
-      </c>
+      <c r="F45" s="7"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B46" t="s">
-        <v>110</v>
+        <v>161</v>
       </c>
       <c r="C46" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E46" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>113</v>
+        <v>162</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2671,33 +2704,33 @@
         <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>167</v>
+        <v>110</v>
       </c>
       <c r="C47" t="s">
-        <v>168</v>
+        <v>114</v>
       </c>
       <c r="E47" t="s">
+        <v>112</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="B48" t="s">
+        <v>165</v>
+      </c>
+      <c r="C48" t="s">
+        <v>166</v>
+      </c>
+      <c r="E48" t="s">
         <v>109</v>
       </c>
-      <c r="F47" s="7" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>1</v>
-      </c>
-      <c r="B49" t="s">
-        <v>129</v>
-      </c>
-      <c r="E49" t="s">
-        <v>140</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>179</v>
-      </c>
-      <c r="K49" s="7" t="s">
-        <v>175</v>
+      <c r="F48" s="7" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
@@ -2705,26 +2738,38 @@
         <v>1</v>
       </c>
       <c r="B50" t="s">
-        <v>177</v>
+        <v>129</v>
       </c>
       <c r="E50" t="s">
+        <v>140</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="K50" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="B51" t="s">
+        <v>173</v>
+      </c>
+      <c r="E51" t="s">
         <v>139</v>
       </c>
-      <c r="F50" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="K50" s="7" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B52" s="5" t="s">
+      <c r="F51" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="K51" s="7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B53" s="5" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B54" s="9" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
@@ -2734,46 +2779,22 @@
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B56" s="9" t="s">
-        <v>173</v>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B57" s="9" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
+      <c r="B58" s="9" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
         <v>125</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>1</v>
-      </c>
-      <c r="B59" t="s">
-        <v>126</v>
-      </c>
-      <c r="C59" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="L59" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="O59" s="7" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>1</v>
-      </c>
-      <c r="B60" t="s">
-        <v>127</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="L60" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="O60" s="7" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
@@ -2781,16 +2802,16 @@
         <v>1</v>
       </c>
       <c r="B61" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="L61" s="4" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="O61" s="7" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
@@ -2798,24 +2819,58 @@
         <v>1</v>
       </c>
       <c r="B62" t="s">
+        <v>127</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="L62" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="O62" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>1</v>
+      </c>
+      <c r="B63" t="s">
+        <v>128</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="L63" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="O63" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>1</v>
+      </c>
+      <c r="B64" t="s">
         <v>138</v>
       </c>
-      <c r="C62" s="7" t="s">
+      <c r="C64" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="L62" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="O62" s="7" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B64" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="E64" s="4" t="s">
-        <v>172</v>
+      <c r="L64" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="O64" s="7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2829,45 +2884,46 @@
     <hyperlink ref="F14" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="F15" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="F16" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="F17" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="F18" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="F19" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="F20" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="F22" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="F23" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="F24" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="F31" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="F32" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="F33" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="F34" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="F35" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="F36" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="C59" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="C60" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="C61" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="F39" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="F40" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="F41" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="C62" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="F38" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="F26" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="F46" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="F42" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="F45" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="F47" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="F50" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="F21" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="K50" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="F49" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="K49" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="O62" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="O59" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="O60" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="O61" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="F2" r:id="rId45" xr:uid="{DD0C5450-CE7D-49B7-8A3D-BBCECC2ABEC5}"/>
+    <hyperlink ref="F19" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="F20" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="F21" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="F23" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="F24" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="F25" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="F32" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="F33" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="F34" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="F35" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="F36" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="F37" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="C61" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="C62" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="C63" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="F40" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="F41" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="F42" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="C64" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="F39" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="F27" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="F47" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="F43" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="F46" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="F48" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="F51" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="F22" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="K51" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="F50" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="K50" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="O64" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="O61" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="O62" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="O63" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="F2" r:id="rId44" xr:uid="{DD0C5450-CE7D-49B7-8A3D-BBCECC2ABEC5}"/>
+    <hyperlink ref="F17" r:id="rId45" xr:uid="{940EE9BC-3C2B-4660-9EEC-D5A03BCC54A3}"/>
+    <hyperlink ref="F18" r:id="rId46" xr:uid="{38F3C576-E9F4-4E09-ADFC-99DBEE708395}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId46"/>
-  <drawing r:id="rId47"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId47"/>
+  <drawing r:id="rId48"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Remove printed washers as requirement for switches.
</commit_message>
<xml_diff>
--- a/Modules/Nucleus/Nucleus_BOM.xlsx
+++ b/Modules/Nucleus/Nucleus_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My-Dev\Modular Synth\Avalon Harmonics\Nucleus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF773A1E-9A66-4EEC-A08E-62B88DBCD6F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A03278-37CB-4B01-98A4-6118B121078E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="190">
   <si>
     <t>Qty</t>
   </si>
@@ -132,9 +132,6 @@
   </si>
   <si>
     <t>Resistor THT</t>
-  </si>
-  <si>
-    <t>Sub-Mini SPDT</t>
   </si>
   <si>
     <t>SW_ON</t>
@@ -627,9 +624,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>Sub-Mini Washer</t>
-  </si>
-  <si>
     <t>Geiger Tube</t>
   </si>
   <si>
@@ -679,9 +673,6 @@
   </si>
   <si>
     <t>https://github.com/Thorinair/Avalon-Harmonics/blob/master/Modules/Nucleus/printable/Nucleus_Back.stl</t>
-  </si>
-  <si>
-    <t>https://github.com/Thorinair/Avalon-Harmonics/blob/master/Misc/Modular_Washers/printable/Modular_Washers__SubMini_Switch.stl</t>
   </si>
   <si>
     <t>https://www.thonk.co.uk/shop/eurorack-diy-essentials/</t>
@@ -758,9 +749,6 @@
   </si>
   <si>
     <t>https://avalonharmonics.etsy.com/listing/1627685702/printed-parts-avalon-harmonics-nucleus</t>
-  </si>
-  <si>
-    <t>https://avalonharmonics.etsy.com/uk/listing/1640523986/printed-parts-20x-submini-switch-washers</t>
   </si>
   <si>
     <t>R1</t>
@@ -789,25 +777,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>Fuse Holder</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>****</t>
-    </r>
-  </si>
-  <si>
-    <t>**** The end stoppers on the fuse holders need to be cut off with flush cutters. This saves 1.4mm of vertical internal height, making the module easier to install. The leg on the side of the cut should be removed too. See photo below!</t>
-  </si>
-  <si>
     <t>*** One LED is used for the printed case.</t>
   </si>
   <si>
@@ -839,6 +808,43 @@
   </si>
   <si>
     <t>https://www.tme.eu/hr/en/details/zl201-40g/pin-headers/connfly/ds1021-1-40sf11-b/</t>
+  </si>
+  <si>
+    <r>
+      <t>Fuse Holder</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*****</t>
+    </r>
+  </si>
+  <si>
+    <t>***** The end stoppers on the fuse holders need to be cut off with flush cutters. This saves 1.4mm of vertical internal height, making the module easier to install. The leg on the side of the cut should be removed too. See photo below!</t>
+  </si>
+  <si>
+    <t>**** Use the included extra nut as a washer between the switch and the panel.</t>
+  </si>
+  <si>
+    <r>
+      <t>Sub-Mini SPDT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>****</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1875,8 +1881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K54" sqref="K54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1906,7 +1912,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1920,13 +1926,13 @@
         <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E2" t="s">
         <v>32</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1940,13 +1946,13 @@
         <v>30</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E3" t="s">
         <v>32</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1960,13 +1966,13 @@
         <v>30</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E4" t="s">
         <v>32</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1980,13 +1986,13 @@
         <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E5" t="s">
         <v>32</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2000,13 +2006,13 @@
         <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E6" t="s">
         <v>32</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2026,7 +2032,7 @@
         <v>32</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2037,16 +2043,16 @@
         <v>16</v>
       </c>
       <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" t="s">
         <v>36</v>
       </c>
-      <c r="D8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" t="s">
-        <v>37</v>
-      </c>
       <c r="F8" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2057,16 +2063,16 @@
         <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2077,16 +2083,16 @@
         <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2097,16 +2103,16 @@
         <v>8</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2117,16 +2123,16 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2137,16 +2143,16 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" t="s">
         <v>45</v>
       </c>
-      <c r="E13" t="s">
-        <v>46</v>
-      </c>
       <c r="F13" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2157,16 +2163,16 @@
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2174,19 +2180,19 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" t="s">
         <v>60</v>
       </c>
-      <c r="D15" t="s">
-        <v>73</v>
-      </c>
-      <c r="E15" t="s">
-        <v>61</v>
-      </c>
       <c r="F15" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -2194,19 +2200,19 @@
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -2214,19 +2220,19 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D17" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="E17" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2237,16 +2243,16 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="E18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -2257,16 +2263,16 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -2277,16 +2283,16 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E20" t="s">
         <v>20</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -2297,16 +2303,16 @@
         <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -2317,16 +2323,16 @@
         <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E22" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -2334,19 +2340,19 @@
         <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E23" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -2354,19 +2360,19 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C24" t="s">
+        <v>189</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="E24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2374,10 +2380,10 @@
         <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>23</v>
@@ -2386,7 +2392,7 @@
         <v>24</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2394,10 +2400,10 @@
         <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D26" t="s">
         <v>26</v>
@@ -2406,7 +2412,7 @@
         <v>25</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2414,10 +2420,10 @@
         <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>29</v>
@@ -2426,7 +2432,7 @@
         <v>25</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -2434,10 +2440,10 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D28" t="s">
         <v>27</v>
@@ -2446,7 +2452,7 @@
         <v>25</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -2454,10 +2460,10 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D29" t="s">
         <v>28</v>
@@ -2466,7 +2472,7 @@
         <v>25</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -2474,10 +2480,10 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D30" t="s">
         <v>22</v>
@@ -2491,16 +2497,16 @@
         <v>2</v>
       </c>
       <c r="B32" t="s">
+        <v>96</v>
+      </c>
+      <c r="C32" t="s">
         <v>97</v>
       </c>
-      <c r="C32" t="s">
+      <c r="E32" t="s">
         <v>98</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" s="7" t="s">
         <v>99</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2508,16 +2514,16 @@
         <v>2</v>
       </c>
       <c r="B33" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" t="s">
         <v>101</v>
       </c>
-      <c r="C33" t="s">
+      <c r="E33" t="s">
         <v>102</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="F33" s="7" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -2525,16 +2531,16 @@
         <v>2</v>
       </c>
       <c r="B34" t="s">
+        <v>104</v>
+      </c>
+      <c r="C34" t="s">
         <v>105</v>
       </c>
-      <c r="C34" t="s">
+      <c r="E34" t="s">
         <v>106</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" s="7" t="s">
         <v>107</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -2542,16 +2548,16 @@
         <v>4</v>
       </c>
       <c r="B35" t="s">
+        <v>114</v>
+      </c>
+      <c r="C35" t="s">
         <v>115</v>
       </c>
-      <c r="C35" t="s">
+      <c r="E35" t="s">
+        <v>118</v>
+      </c>
+      <c r="F35" s="7" t="s">
         <v>116</v>
-      </c>
-      <c r="E35" t="s">
-        <v>119</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2559,16 +2565,16 @@
         <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C36" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E36" t="s">
+        <v>119</v>
+      </c>
+      <c r="F36" s="7" t="s">
         <v>120</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2576,16 +2582,16 @@
         <v>4</v>
       </c>
       <c r="B37" t="s">
+        <v>121</v>
+      </c>
+      <c r="C37" t="s">
+        <v>115</v>
+      </c>
+      <c r="E37" t="s">
         <v>122</v>
       </c>
-      <c r="C37" t="s">
-        <v>116</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="F37" s="7" t="s">
         <v>123</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -2596,16 +2602,16 @@
         <v>1</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C39" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E39" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2613,16 +2619,16 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C40" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E40" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2630,16 +2636,16 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C41" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E41" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -2647,16 +2653,16 @@
         <v>5</v>
       </c>
       <c r="B42" t="s">
+        <v>134</v>
+      </c>
+      <c r="C42" t="s">
+        <v>132</v>
+      </c>
+      <c r="E42" t="s">
         <v>135</v>
       </c>
-      <c r="C42" t="s">
-        <v>133</v>
-      </c>
-      <c r="E42" t="s">
-        <v>136</v>
-      </c>
       <c r="F42" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -2664,30 +2670,30 @@
         <v>2</v>
       </c>
       <c r="B43" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C43" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E43" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B44" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C44" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E44" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F44" s="7"/>
     </row>
@@ -2699,16 +2705,16 @@
         <v>3</v>
       </c>
       <c r="B46" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E46" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2716,16 +2722,16 @@
         <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C47" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E47" t="s">
+        <v>111</v>
+      </c>
+      <c r="F47" s="7" t="s">
         <v>112</v>
-      </c>
-      <c r="F47" s="7" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -2733,16 +2739,16 @@
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C48" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E48" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
@@ -2750,16 +2756,16 @@
         <v>1</v>
       </c>
       <c r="B50" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E50" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="K50" s="7" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
@@ -2767,63 +2773,51 @@
         <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E51" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="K51" s="7" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B53" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B55" s="9" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B56" s="9" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B57" s="9" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B58" s="9" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
-        <v>125</v>
+        <v>188</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B59" s="9" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>1</v>
-      </c>
-      <c r="B61" t="s">
-        <v>126</v>
-      </c>
-      <c r="C61" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="L61" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="O61" s="7" t="s">
-        <v>177</v>
+      <c r="A61" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
@@ -2831,16 +2825,16 @@
         <v>1</v>
       </c>
       <c r="B62" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L62" s="4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="O62" s="7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
@@ -2848,16 +2842,16 @@
         <v>1</v>
       </c>
       <c r="B63" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="L63" s="4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="O63" s="7" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
@@ -2865,24 +2859,24 @@
         <v>1</v>
       </c>
       <c r="B64" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="L64" s="4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="O64" s="7" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -2908,37 +2902,35 @@
     <hyperlink ref="F35" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
     <hyperlink ref="F36" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
     <hyperlink ref="F37" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="C61" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="C62" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="C63" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="C62" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="C63" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="C64" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
     <hyperlink ref="F40" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
     <hyperlink ref="F41" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
     <hyperlink ref="F42" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="C64" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="F39" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="F27" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="F47" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="F43" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="F46" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="F48" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="F51" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="F22" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="K51" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="F50" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="K50" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="O64" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="O61" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="O62" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="O63" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="F2" r:id="rId44" xr:uid="{DD0C5450-CE7D-49B7-8A3D-BBCECC2ABEC5}"/>
-    <hyperlink ref="F17" r:id="rId45" xr:uid="{940EE9BC-3C2B-4660-9EEC-D5A03BCC54A3}"/>
-    <hyperlink ref="F18" r:id="rId46" xr:uid="{38F3C576-E9F4-4E09-ADFC-99DBEE708395}"/>
-    <hyperlink ref="F26" r:id="rId47" xr:uid="{13CDBD9F-609D-4DBD-97BE-822003C4B835}"/>
-    <hyperlink ref="F28" r:id="rId48" xr:uid="{18F71FC3-BB9D-4329-A570-6693B623435A}"/>
-    <hyperlink ref="F29" r:id="rId49" xr:uid="{7FBCA6ED-A9F0-4C0E-BDD4-980D2C9B7AEC}"/>
+    <hyperlink ref="F39" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="F27" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="F47" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="F43" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="F46" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="F48" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="F51" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="F22" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="K51" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="F50" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="K50" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="O62" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="O63" r:id="rId40" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="O64" r:id="rId41" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="F2" r:id="rId42" xr:uid="{DD0C5450-CE7D-49B7-8A3D-BBCECC2ABEC5}"/>
+    <hyperlink ref="F17" r:id="rId43" xr:uid="{940EE9BC-3C2B-4660-9EEC-D5A03BCC54A3}"/>
+    <hyperlink ref="F18" r:id="rId44" xr:uid="{38F3C576-E9F4-4E09-ADFC-99DBEE708395}"/>
+    <hyperlink ref="F26" r:id="rId45" xr:uid="{13CDBD9F-609D-4DBD-97BE-822003C4B835}"/>
+    <hyperlink ref="F28" r:id="rId46" xr:uid="{18F71FC3-BB9D-4329-A570-6693B623435A}"/>
+    <hyperlink ref="F29" r:id="rId47" xr:uid="{7FBCA6ED-A9F0-4C0E-BDD4-980D2C9B7AEC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId50"/>
-  <drawing r:id="rId51"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId48"/>
+  <drawing r:id="rId49"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change pot and knob on Nucleus for Thonk one.
</commit_message>
<xml_diff>
--- a/Modules/Nucleus/Nucleus_BOM.xlsx
+++ b/Modules/Nucleus/Nucleus_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My-Dev\Modular Synth\Avalon Harmonics\Nucleus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1552A3-DA7D-40E6-B567-8E0EDEA5E92C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AEEE247-F616-4AA8-B01F-B317C1D07574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -706,22 +706,7 @@
     <t>https://pushermanproductions.com/product/pushernuts-gold-smooth-edge-jack-nuts-pack-of-25/</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/32965476651.html</t>
-  </si>
-  <si>
     <t>https://www.ebay.co.uk/itm/185419609093</t>
-  </si>
-  <si>
-    <t>Black 6.35mm-Round</t>
-  </si>
-  <si>
-    <t>Aliexpress Knob 15mm</t>
-  </si>
-  <si>
-    <t>Pot 9mm Alpha 6.35mm</t>
-  </si>
-  <si>
-    <t>https://www.thonk.co.uk/shop/alpha-9mm-pots/</t>
   </si>
   <si>
     <t>Wiring Diagram</t>
@@ -848,6 +833,21 @@
   </si>
   <si>
     <t>https://www.tme.eu/hr/en/details/zl202-80g/pin-headers/connfly/ds1021-2-40sf11/</t>
+  </si>
+  <si>
+    <t>Black D-Shaft Line</t>
+  </si>
+  <si>
+    <t>https://www.thonk.co.uk/shop/bastl-knobs/</t>
+  </si>
+  <si>
+    <t>Bastl Style Alu Knob 15mm</t>
+  </si>
+  <si>
+    <t>Pot 9mm Alpha D-Shaft</t>
+  </si>
+  <si>
+    <t>https://www.thonk.co.uk/shop/alpha-9mm-pots-dshaft/</t>
   </si>
 </sst>
 </file>
@@ -1884,8 +1884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1929,7 +1929,7 @@
         <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E2" t="s">
         <v>32</v>
@@ -1949,7 +1949,7 @@
         <v>30</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E3" t="s">
         <v>32</v>
@@ -2223,19 +2223,19 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C17" t="s">
         <v>57</v>
       </c>
       <c r="D17" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="E17" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2249,7 +2249,7 @@
         <v>57</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E18" t="s">
         <v>54</v>
@@ -2326,7 +2326,7 @@
         <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>164</v>
+        <v>189</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>49</v>
@@ -2335,7 +2335,7 @@
         <v>142</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>165</v>
+        <v>190</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -2349,7 +2349,7 @@
         <v>47</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="E23" t="s">
         <v>156</v>
@@ -2366,7 +2366,7 @@
         <v>65</v>
       </c>
       <c r="C24" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>33</v>
@@ -2415,7 +2415,7 @@
         <v>25</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -2455,7 +2455,7 @@
         <v>25</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -2475,7 +2475,7 @@
         <v>25</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -2495,7 +2495,7 @@
         <v>25</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -2679,13 +2679,13 @@
         <v>149</v>
       </c>
       <c r="C43" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="E43" t="s">
         <v>150</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -2745,16 +2745,16 @@
         <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>162</v>
+        <v>186</v>
       </c>
       <c r="C48" t="s">
-        <v>163</v>
+        <v>188</v>
       </c>
       <c r="E48" t="s">
         <v>108</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>160</v>
+        <v>187</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
@@ -2768,10 +2768,10 @@
         <v>138</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="K50" s="7" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
@@ -2779,16 +2779,16 @@
         <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E51" t="s">
         <v>137</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K51" s="7" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
@@ -2803,22 +2803,22 @@
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B56" s="9" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B57" s="9" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B58" s="9" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B59" s="9" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
@@ -2837,10 +2837,10 @@
         <v>151</v>
       </c>
       <c r="L62" s="4" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="O62" s="7" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
@@ -2854,10 +2854,10 @@
         <v>152</v>
       </c>
       <c r="L63" s="4" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="O63" s="7" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
@@ -2871,18 +2871,18 @@
         <v>153</v>
       </c>
       <c r="L64" s="4" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="O64" s="7" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="4" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -2919,22 +2919,22 @@
     <hyperlink ref="F47" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
     <hyperlink ref="F43" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
     <hyperlink ref="F46" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="F48" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="F51" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="F22" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="K51" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="F50" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="K50" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="O62" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="O63" r:id="rId40" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="O64" r:id="rId41" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="F2" r:id="rId42" xr:uid="{DD0C5450-CE7D-49B7-8A3D-BBCECC2ABEC5}"/>
-    <hyperlink ref="F17" r:id="rId43" xr:uid="{940EE9BC-3C2B-4660-9EEC-D5A03BCC54A3}"/>
-    <hyperlink ref="F18" r:id="rId44" xr:uid="{38F3C576-E9F4-4E09-ADFC-99DBEE708395}"/>
-    <hyperlink ref="F26" r:id="rId45" xr:uid="{13CDBD9F-609D-4DBD-97BE-822003C4B835}"/>
-    <hyperlink ref="F28" r:id="rId46" xr:uid="{18F71FC3-BB9D-4329-A570-6693B623435A}"/>
-    <hyperlink ref="F29" r:id="rId47" xr:uid="{7FBCA6ED-A9F0-4C0E-BDD4-980D2C9B7AEC}"/>
-    <hyperlink ref="F30" r:id="rId48" xr:uid="{0A7E4D8D-669F-4DF0-965E-6BED00A668C1}"/>
+    <hyperlink ref="F51" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="K51" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="F50" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="K50" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="O62" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="O63" r:id="rId38" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="O64" r:id="rId39" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="F2" r:id="rId40" xr:uid="{DD0C5450-CE7D-49B7-8A3D-BBCECC2ABEC5}"/>
+    <hyperlink ref="F17" r:id="rId41" xr:uid="{940EE9BC-3C2B-4660-9EEC-D5A03BCC54A3}"/>
+    <hyperlink ref="F18" r:id="rId42" xr:uid="{38F3C576-E9F4-4E09-ADFC-99DBEE708395}"/>
+    <hyperlink ref="F26" r:id="rId43" xr:uid="{13CDBD9F-609D-4DBD-97BE-822003C4B835}"/>
+    <hyperlink ref="F28" r:id="rId44" xr:uid="{18F71FC3-BB9D-4329-A570-6693B623435A}"/>
+    <hyperlink ref="F29" r:id="rId45" xr:uid="{7FBCA6ED-A9F0-4C0E-BDD4-980D2C9B7AEC}"/>
+    <hyperlink ref="F30" r:id="rId46" xr:uid="{0A7E4D8D-669F-4DF0-965E-6BED00A668C1}"/>
+    <hyperlink ref="F48" r:id="rId47" xr:uid="{C637B40B-75E7-4AD6-9CA4-5BD086BF954E}"/>
+    <hyperlink ref="F22" r:id="rId48" xr:uid="{78D2B6DC-3673-4D93-8128-FA4E104975E9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId49"/>

</xml_diff>